<commit_message>
Added features of some paper and updated importance column
</commit_message>
<xml_diff>
--- a/ObjDetection.xlsx
+++ b/ObjDetection.xlsx
@@ -5,22 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rough\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Project-350\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765DAFCB-ED2A-4EEB-9CC2-C9DE93F29332}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EDADFC-2AC0-46DD-863F-4C13F32E47FE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="31125" yWindow="2115" windowWidth="16365" windowHeight="8595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="4" r:id="rId1"/>
     <sheet name="System" sheetId="3" r:id="rId2"/>
     <sheet name="DL_later" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1227,7 +1233,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>